<commit_message>
cambio de resultados esperados en caso de prueba 1
</commit_message>
<xml_diff>
--- a/Test_cases/caso de prueba 1.xlsx
+++ b/Test_cases/caso de prueba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moren\Documents\GitHub\Grupo0102\Test_cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lautaroacosta/Documents/Facultad/Testing/Grupo0102/Test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA70FC7-0B98-403C-A91C-F89FE5656E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD985614-D2BC-3F4E-9F0C-A10B7B4591D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="760" windowWidth="30060" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>Click register</t>
   </si>
   <si>
-    <t>Customer is logged in</t>
-  </si>
-  <si>
     <t>User create account (Alternative Scenario)</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>PE-16</t>
+  </si>
+  <si>
+    <t>El usuario pueda registrarse para luego iniciar sesion</t>
   </si>
 </sst>
 </file>
@@ -836,47 +836,47 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,18 +1097,18 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="157" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,12 +1118,12 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -1132,7 +1132,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1146,8 +1146,8 @@
         <v>7</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1156,7 +1156,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1196,7 +1196,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1230,8 +1230,8 @@
       <c r="E6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1240,7 +1240,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
@@ -1254,8 +1254,8 @@
       <c r="E7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1264,7 +1264,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>1</v>
       </c>
@@ -1278,8 +1278,8 @@
       <c r="E8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1288,7 +1288,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>2</v>
       </c>
@@ -1302,8 +1302,8 @@
       <c r="E9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1312,7 +1312,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>3</v>
       </c>
@@ -1326,8 +1326,8 @@
       <c r="E10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1336,7 +1336,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>4</v>
       </c>
@@ -1360,7 +1360,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
       <c r="B12" s="11"/>
       <c r="C12" s="4"/>
@@ -1370,8 +1370,8 @@
       <c r="E12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1380,7 +1380,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="D13" s="17">
         <v>8</v>
@@ -1398,7 +1398,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="D14" s="17">
         <v>9</v>
@@ -1407,18 +1407,18 @@
         <v>28</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="53"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="50"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" s="17">
         <v>10</v>
       </c>
@@ -1426,24 +1426,24 @@
         <v>30</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54" t="s">
+      <c r="H15" s="50"/>
+      <c r="I15" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="53"/>
-      <c r="K15" s="54" t="s">
+      <c r="J15" s="50"/>
+      <c r="K15" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="53"/>
-      <c r="M15" s="54" t="s">
+      <c r="L15" s="50"/>
+      <c r="M15" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="53"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="50"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D16" s="17">
         <v>11</v>
       </c>
@@ -1451,24 +1451,24 @@
         <v>35</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="54" t="s">
+      <c r="H16" s="51"/>
+      <c r="I16" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="54" t="s">
+      <c r="J16" s="51"/>
+      <c r="K16" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="52"/>
-      <c r="M16" s="54" t="s">
+      <c r="L16" s="51"/>
+      <c r="M16" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="52"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="51"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="17">
         <v>12</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D18" s="17">
         <v>13</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D19" s="17">
         <v>14</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F20" s="4"/>
       <c r="G20" s="26" t="s">
         <v>44</v>
@@ -1588,7 +1588,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F21" s="4"/>
       <c r="G21" s="26" t="s">
         <v>44</v>
@@ -1611,7 +1611,7 @@
       <c r="M21" s="29"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F22" s="4"/>
       <c r="G22" s="26" t="s">
         <v>44</v>
@@ -1634,7 +1634,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F23" s="4"/>
       <c r="G23" s="26" t="s">
         <v>44</v>
@@ -1657,7 +1657,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="26" t="s">
         <v>44</v>
       </c>
@@ -1679,16 +1679,16 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="4"/>
       <c r="G25" s="26" t="s">
         <v>44</v>
@@ -1709,12 +1709,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="40"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="4"/>
       <c r="G26" s="26" t="s">
         <v>44</v>
@@ -1735,12 +1735,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="31" t="s">
@@ -1769,7 +1769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1795,18 +1795,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="57" t="s">
+      <c r="C29" s="48"/>
+      <c r="D29" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="50"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="4"/>
       <c r="G29" s="26" t="s">
         <v>44</v>
@@ -1827,290 +1827,290 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36">
         <v>1</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="43" t="s">
+      <c r="C30" s="42"/>
+      <c r="D30" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="36">
         <v>2</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="43" t="s">
+      <c r="C31" s="42"/>
+      <c r="D31" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="39"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E31" s="42"/>
+    </row>
+    <row r="32" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="36">
         <v>3</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="43" t="s">
+      <c r="C32" s="42"/>
+      <c r="D32" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="39"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E32" s="42"/>
+    </row>
+    <row r="33" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="36">
         <v>4</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="43" t="s">
+      <c r="C33" s="42"/>
+      <c r="D33" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="39"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E33" s="42"/>
+    </row>
+    <row r="34" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="36">
         <v>5</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="43" t="s">
+      <c r="C34" s="42"/>
+      <c r="D34" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="39"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E34" s="42"/>
+    </row>
+    <row r="35" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="36">
         <v>6</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="43" t="s">
+      <c r="C35" s="42"/>
+      <c r="D35" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="39"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E35" s="42"/>
+    </row>
+    <row r="36" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="36">
         <v>7</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="43" t="s">
+      <c r="C36" s="42"/>
+      <c r="D36" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="39"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E36" s="42"/>
+    </row>
+    <row r="37" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="36">
         <v>8</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="43" t="s">
+      <c r="C37" s="42"/>
+      <c r="D37" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="39"/>
-    </row>
-    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E37" s="42"/>
+    </row>
+    <row r="38" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="36">
         <v>9</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="43" t="s">
+      <c r="C38" s="42"/>
+      <c r="D38" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E38" s="42"/>
+    </row>
+    <row r="39" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="36">
         <v>10</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="43" t="s">
+      <c r="C39" s="42"/>
+      <c r="D39" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="39"/>
-    </row>
-    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E39" s="42"/>
+    </row>
+    <row r="40" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="36">
         <v>11</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="43" t="s">
+      <c r="C40" s="42"/>
+      <c r="D40" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="39"/>
-    </row>
-    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E40" s="42"/>
+    </row>
+    <row r="41" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="36">
         <v>12</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="39"/>
-      <c r="D41" s="43" t="s">
+      <c r="C41" s="42"/>
+      <c r="D41" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="39"/>
-    </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="E41" s="42"/>
+    </row>
+    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="36">
         <v>13</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="43" t="s">
+      <c r="C42" s="42"/>
+      <c r="D42" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="G42" s="38" t="s">
+      <c r="E42" s="42"/>
+      <c r="G42" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="H42" s="39"/>
-      <c r="I42" s="38" t="s">
+      <c r="H42" s="42"/>
+      <c r="I42" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="J42" s="39"/>
-      <c r="K42" s="38" t="s">
+      <c r="J42" s="42"/>
+      <c r="K42" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="L42" s="39"/>
-      <c r="M42" s="38" t="s">
+      <c r="L42" s="42"/>
+      <c r="M42" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="N42" s="39"/>
-    </row>
-    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="N42" s="42"/>
+    </row>
+    <row r="43" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A43" s="36">
         <v>14</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="43" t="s">
+      <c r="C43" s="42"/>
+      <c r="D43" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="42" t="s">
+      <c r="E43" s="42"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="J43" s="39"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="41"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="41"/>
-    </row>
-    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="J43" s="42"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="56"/>
+    </row>
+    <row r="44" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="36">
         <v>15</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="43" t="s">
+      <c r="C44" s="42"/>
+      <c r="D44" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="42"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="56"/>
+    </row>
+    <row r="45" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="G45" s="55"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="55"/>
+      <c r="N45" s="56"/>
+    </row>
+    <row r="46" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="G46" s="55"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="56"/>
+    </row>
+    <row r="47" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="G47" s="55"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="56"/>
+    </row>
+    <row r="48" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+      <c r="A48" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="41"/>
-    </row>
-    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G45" s="40"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="40"/>
-      <c r="N45" s="41"/>
-    </row>
-    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G46" s="40"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="41"/>
-    </row>
-    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="G47" s="40"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="41"/>
-      <c r="M47" s="40"/>
-      <c r="N47" s="41"/>
-    </row>
-    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-    </row>
-    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="56"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-    </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+    </row>
+    <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A49" s="40"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="58" t="s">
-        <v>90</v>
+      <c r="B50" s="38" t="s">
+        <v>89</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="31" t="s">
@@ -2120,129 +2120,116 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="50"/>
-      <c r="D52" s="57" t="s">
+      <c r="C52" s="48"/>
+      <c r="D52" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E52" s="50"/>
-    </row>
-    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E52" s="48"/>
+    </row>
+    <row r="53" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="43" t="s">
+      <c r="E53" s="42"/>
+    </row>
+    <row r="54" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A54" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="39"/>
-    </row>
-    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="36" t="s">
+      <c r="B54" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="43" t="s">
+      <c r="E54" s="42"/>
+    </row>
+    <row r="55" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A55" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="E54" s="39"/>
-    </row>
-    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="36" t="s">
+      <c r="B55" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="C55" s="42"/>
+      <c r="D55" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="43" t="s">
+      <c r="E55" s="42"/>
+    </row>
+    <row r="56" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A56" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E55" s="39"/>
-    </row>
-    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="36" t="s">
+      <c r="B56" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="C56" s="42"/>
+      <c r="D56" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="E56" s="39"/>
-    </row>
-    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E56" s="42"/>
+    </row>
+    <row r="57" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="37"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="47"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:E26"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D42:E42"/>
@@ -2259,38 +2246,51 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:E26"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
     <mergeCell ref="D55:E55"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="B48:E49"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Caso de prueba 1
</commit_message>
<xml_diff>
--- a/Test_cases/caso de prueba 1.xlsx
+++ b/Test_cases/caso de prueba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lautaroacosta/Documents/Facultad/Testing/Grupo0102/Test_cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moren\Documents\GitHub\Grupo0102\Test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD985614-D2BC-3F4E-9F0C-A10B7B4591D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA6B768-ED82-44C5-9923-58E005BD6FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="760" windowWidth="30060" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -292,14 +292,14 @@
     <t>PE-16</t>
   </si>
   <si>
-    <t>El usuario pueda registrarse para luego iniciar sesion</t>
+    <t xml:space="preserve">User can sign up to sign in later </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -408,6 +408,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -737,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -837,46 +851,47 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,18 +1112,18 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="36.5" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,10 +1133,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="46"/>
       <c r="G1" s="46"/>
       <c r="H1" s="4"/>
@@ -1132,7 +1147,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1171,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1195,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1196,7 +1211,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1235,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1240,7 +1255,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>13</v>
       </c>
@@ -1264,7 +1279,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>1</v>
       </c>
@@ -1288,7 +1303,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>2</v>
       </c>
@@ -1312,7 +1327,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>3</v>
       </c>
@@ -1336,7 +1351,7 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>4</v>
       </c>
@@ -1360,7 +1375,7 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="11"/>
       <c r="C12" s="4"/>
@@ -1380,7 +1395,7 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="D13" s="17">
         <v>8</v>
@@ -1398,7 +1413,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="D14" s="17">
         <v>9</v>
@@ -1407,18 +1422,18 @@
         <v>28</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="50"/>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="51"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="17">
         <v>10</v>
       </c>
@@ -1426,24 +1441,24 @@
         <v>30</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="50"/>
-      <c r="I15" s="49" t="s">
+      <c r="H15" s="51"/>
+      <c r="I15" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="50"/>
-      <c r="K15" s="49" t="s">
+      <c r="J15" s="51"/>
+      <c r="K15" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="50"/>
-      <c r="M15" s="49" t="s">
+      <c r="L15" s="51"/>
+      <c r="M15" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="50"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N15" s="51"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="17">
         <v>11</v>
       </c>
@@ -1451,24 +1466,24 @@
         <v>35</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="51"/>
-      <c r="I16" s="49" t="s">
+      <c r="H16" s="50"/>
+      <c r="I16" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="49" t="s">
+      <c r="J16" s="50"/>
+      <c r="K16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="51"/>
-      <c r="M16" s="49" t="s">
+      <c r="L16" s="50"/>
+      <c r="M16" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="51"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N16" s="50"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="17">
         <v>12</v>
       </c>
@@ -1501,7 +1516,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="17">
         <v>13</v>
       </c>
@@ -1532,7 +1547,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="17">
         <v>14</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="4"/>
       <c r="G20" s="26" t="s">
         <v>44</v>
@@ -1588,7 +1603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F21" s="4"/>
       <c r="G21" s="26" t="s">
         <v>44</v>
@@ -1611,7 +1626,7 @@
       <c r="M21" s="29"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="4"/>
       <c r="G22" s="26" t="s">
         <v>44</v>
@@ -1634,7 +1649,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23" s="4"/>
       <c r="G23" s="26" t="s">
         <v>44</v>
@@ -1657,7 +1672,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="26" t="s">
         <v>44</v>
       </c>
@@ -1679,16 +1694,16 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39" t="s">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="4"/>
       <c r="G25" s="26" t="s">
         <v>44</v>
@@ -1709,9 +1724,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
       <c r="E26" s="46"/>
@@ -1735,7 +1750,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>51</v>
       </c>
@@ -1769,7 +1784,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1795,7 +1810,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>54</v>
       </c>
@@ -1827,7 +1842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36">
         <v>1</v>
       </c>
@@ -1841,7 +1856,7 @@
       <c r="E30" s="42"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="36">
         <v>2</v>
       </c>
@@ -1854,7 +1869,7 @@
       </c>
       <c r="E31" s="42"/>
     </row>
-    <row r="32" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="36">
         <v>3</v>
       </c>
@@ -1867,7 +1882,7 @@
       </c>
       <c r="E32" s="42"/>
     </row>
-    <row r="33" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36">
         <v>4</v>
       </c>
@@ -1880,7 +1895,7 @@
       </c>
       <c r="E33" s="42"/>
     </row>
-    <row r="34" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="36">
         <v>5</v>
       </c>
@@ -1893,7 +1908,7 @@
       </c>
       <c r="E34" s="42"/>
     </row>
-    <row r="35" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="36">
         <v>6</v>
       </c>
@@ -1906,7 +1921,7 @@
       </c>
       <c r="E35" s="42"/>
     </row>
-    <row r="36" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="36">
         <v>7</v>
       </c>
@@ -1919,7 +1934,7 @@
       </c>
       <c r="E36" s="42"/>
     </row>
-    <row r="37" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="36">
         <v>8</v>
       </c>
@@ -1932,7 +1947,7 @@
       </c>
       <c r="E37" s="42"/>
     </row>
-    <row r="38" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="36">
         <v>9</v>
       </c>
@@ -1945,7 +1960,7 @@
       </c>
       <c r="E38" s="42"/>
     </row>
-    <row r="39" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="36">
         <v>10</v>
       </c>
@@ -1958,7 +1973,7 @@
       </c>
       <c r="E39" s="42"/>
     </row>
-    <row r="40" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="36">
         <v>11</v>
       </c>
@@ -1971,7 +1986,7 @@
       </c>
       <c r="E40" s="42"/>
     </row>
-    <row r="41" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="36">
         <v>12</v>
       </c>
@@ -1984,7 +1999,7 @@
       </c>
       <c r="E41" s="42"/>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>13</v>
       </c>
@@ -1996,24 +2011,24 @@
         <v>60</v>
       </c>
       <c r="E42" s="42"/>
-      <c r="G42" s="57" t="s">
+      <c r="G42" s="43" t="s">
         <v>72</v>
       </c>
       <c r="H42" s="42"/>
-      <c r="I42" s="57" t="s">
+      <c r="I42" s="43" t="s">
         <v>72</v>
       </c>
       <c r="J42" s="42"/>
-      <c r="K42" s="57" t="s">
+      <c r="K42" s="43" t="s">
         <v>72</v>
       </c>
       <c r="L42" s="42"/>
-      <c r="M42" s="57" t="s">
+      <c r="M42" s="43" t="s">
         <v>72</v>
       </c>
       <c r="N42" s="42"/>
     </row>
-    <row r="43" spans="1:14" ht="14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="36">
         <v>14</v>
       </c>
@@ -2025,18 +2040,18 @@
         <v>60</v>
       </c>
       <c r="E43" s="42"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="58" t="s">
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="44" t="s">
         <v>74</v>
       </c>
       <c r="J43" s="42"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="55"/>
-      <c r="N43" s="56"/>
-    </row>
-    <row r="44" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="K43" s="39"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="40"/>
+    </row>
+    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="36">
         <v>15</v>
       </c>
@@ -2048,64 +2063,66 @@
         <v>90</v>
       </c>
       <c r="E44" s="42"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="55"/>
-      <c r="N44" s="56"/>
-    </row>
-    <row r="45" spans="1:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="G45" s="55"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="56"/>
-    </row>
-    <row r="46" spans="1:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="G46" s="55"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="55"/>
-      <c r="N46" s="56"/>
-    </row>
-    <row r="47" spans="1:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="G47" s="55"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="55"/>
-      <c r="N47" s="56"/>
-    </row>
-    <row r="48" spans="1:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="39" t="s">
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="40"/>
+    </row>
+    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="40"/>
+    </row>
+    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E46" s="41"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="40"/>
+    </row>
+    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="40"/>
+    </row>
+    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-    </row>
-    <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="40"/>
-      <c r="B49" s="45"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+    </row>
+    <row r="49" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="54"/>
+      <c r="B49" s="57"/>
       <c r="C49" s="46"/>
       <c r="D49" s="46"/>
       <c r="E49" s="46"/>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>51</v>
       </c>
@@ -2120,14 +2137,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
         <v>54</v>
       </c>
@@ -2140,7 +2157,7 @@
       </c>
       <c r="E52" s="48"/>
     </row>
-    <row r="53" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>77</v>
       </c>
@@ -2153,7 +2170,7 @@
       </c>
       <c r="E53" s="42"/>
     </row>
-    <row r="54" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
         <v>80</v>
       </c>
@@ -2166,7 +2183,7 @@
       </c>
       <c r="E54" s="42"/>
     </row>
-    <row r="55" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="36" t="s">
         <v>83</v>
       </c>
@@ -2179,7 +2196,7 @@
       </c>
       <c r="E55" s="42"/>
     </row>
-    <row r="56" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="36" t="s">
         <v>86</v>
       </c>
@@ -2192,78 +2209,30 @@
       </c>
       <c r="E56" s="42"/>
     </row>
-    <row r="57" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="37"/>
-      <c r="B57" s="54"/>
+      <c r="B57" s="45"/>
       <c r="C57" s="46"/>
-      <c r="D57" s="54"/>
+      <c r="D57" s="45"/>
       <c r="E57" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
+  <mergeCells count="91">
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B48:E49"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:E26"/>
     <mergeCell ref="D29:E29"/>
@@ -2276,21 +2245,70 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B48:E49"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>